<commit_message>
Priya worked on delevery location and vebdor list page
</commit_message>
<xml_diff>
--- a/Documents/Images and productList/ProductList.xlsx
+++ b/Documents/Images and productList/ProductList.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$AE$323</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$AE$323</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -5202,23 +5202,23 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>720</xdr:colOff>
       <xdr:row>259</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
+      <xdr:colOff>150120</xdr:colOff>
       <xdr:row>259</xdr:row>
       <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11689560" y="539280"/>
-          <a:ext cx="150120" cy="150120"/>
+          <a:off x="11691000" y="421719480"/>
+          <a:ext cx="149400" cy="149400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5242,23 +5242,23 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>720</xdr:colOff>
       <xdr:row>259</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
+      <xdr:colOff>150120</xdr:colOff>
       <xdr:row>259</xdr:row>
       <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="1" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11689560" y="539280"/>
-          <a:ext cx="150120" cy="150120"/>
+          <a:off x="11691000" y="421719480"/>
+          <a:ext cx="149400" cy="149400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5282,23 +5282,23 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>720</xdr:colOff>
       <xdr:row>259</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
+      <xdr:colOff>150120</xdr:colOff>
       <xdr:row>259</xdr:row>
       <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11689560" y="539280"/>
-          <a:ext cx="150120" cy="150120"/>
+          <a:off x="11691000" y="421719480"/>
+          <a:ext cx="149400" cy="149400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5322,13 +5322,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMI323"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A260" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F260" activeCellId="0" sqref="F260"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B282" activeCellId="0" sqref="B250:B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5474,7 +5474,7 @@
       <c r="AMH1" s="1"/>
       <c r="AMI1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="129.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -5554,7 +5554,7 @@
       <c r="AE2" s="8"/>
       <c r="AF2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -5634,7 +5634,7 @@
       <c r="AE3" s="8"/>
       <c r="AF3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -5712,7 +5712,7 @@
       <c r="AE4" s="8"/>
       <c r="AF4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -5792,7 +5792,7 @@
       <c r="AE5" s="8"/>
       <c r="AF5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="AE6" s="8"/>
       <c r="AF6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -5952,7 +5952,7 @@
       <c r="AE7" s="8"/>
       <c r="AF7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -6032,7 +6032,7 @@
       <c r="AE8" s="8"/>
       <c r="AF8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="AE9" s="8"/>
       <c r="AF9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -6192,7 +6192,7 @@
       <c r="AE10" s="8"/>
       <c r="AF10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
@@ -6272,7 +6272,7 @@
       <c r="AE11" s="8"/>
       <c r="AF11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
@@ -6352,7 +6352,7 @@
       <c r="AE12" s="8"/>
       <c r="AF12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -6432,7 +6432,7 @@
       <c r="AE13" s="8"/>
       <c r="AF13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -6512,7 +6512,7 @@
       <c r="AE14" s="8"/>
       <c r="AF14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
@@ -6592,7 +6592,7 @@
       <c r="AE15" s="8"/>
       <c r="AF15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
@@ -6672,7 +6672,7 @@
       <c r="AE16" s="8"/>
       <c r="AF16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -6752,7 +6752,7 @@
       <c r="AE17" s="8"/>
       <c r="AF17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
@@ -6832,7 +6832,7 @@
       <c r="AE18" s="8"/>
       <c r="AF18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
@@ -6912,7 +6912,7 @@
       <c r="AE19" s="8"/>
       <c r="AF19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
@@ -6992,7 +6992,7 @@
       <c r="AE20" s="8"/>
       <c r="AF20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
@@ -7072,7 +7072,7 @@
       <c r="AE21" s="8"/>
       <c r="AF21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
@@ -7152,7 +7152,7 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
@@ -7232,7 +7232,7 @@
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
@@ -7312,7 +7312,7 @@
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
@@ -7392,7 +7392,7 @@
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
@@ -7472,7 +7472,7 @@
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
@@ -7552,7 +7552,7 @@
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
@@ -7632,7 +7632,7 @@
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
@@ -7712,7 +7712,7 @@
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
@@ -7792,7 +7792,7 @@
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
@@ -7872,7 +7872,7 @@
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
@@ -7952,7 +7952,7 @@
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
@@ -8032,7 +8032,7 @@
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
@@ -8112,7 +8112,7 @@
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
@@ -8192,7 +8192,7 @@
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
@@ -8272,7 +8272,7 @@
       <c r="AE36" s="4"/>
       <c r="AF36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
@@ -8350,7 +8350,7 @@
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
@@ -8430,7 +8430,7 @@
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
@@ -8510,7 +8510,7 @@
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="AE40" s="4"/>
       <c r="AF40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
@@ -8670,7 +8670,7 @@
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
@@ -8750,7 +8750,7 @@
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
@@ -8830,7 +8830,7 @@
       <c r="AE43" s="4"/>
       <c r="AF43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
@@ -8910,7 +8910,7 @@
       <c r="AE44" s="4"/>
       <c r="AF44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
@@ -8990,7 +8990,7 @@
       <c r="AE45" s="4"/>
       <c r="AF45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
@@ -9070,7 +9070,7 @@
       <c r="AE46" s="4"/>
       <c r="AF46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
@@ -9150,7 +9150,7 @@
       <c r="AE47" s="4"/>
       <c r="AF47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
@@ -9230,7 +9230,7 @@
       <c r="AE48" s="4"/>
       <c r="AF48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
@@ -9310,7 +9310,7 @@
       <c r="AE49" s="4"/>
       <c r="AF49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
@@ -9390,7 +9390,7 @@
       <c r="AE50" s="4"/>
       <c r="AF50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
@@ -9470,7 +9470,7 @@
       <c r="AE51" s="4"/>
       <c r="AF51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
@@ -9550,7 +9550,7 @@
       <c r="AE52" s="4"/>
       <c r="AF52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
@@ -9630,7 +9630,7 @@
       <c r="AE53" s="4"/>
       <c r="AF53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
@@ -9710,7 +9710,7 @@
       <c r="AE54" s="4"/>
       <c r="AF54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
@@ -9790,7 +9790,7 @@
       <c r="AE55" s="4"/>
       <c r="AF55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
@@ -9870,7 +9870,7 @@
       <c r="AE56" s="4"/>
       <c r="AF56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
@@ -9950,7 +9950,7 @@
       <c r="AE57" s="4"/>
       <c r="AF57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
@@ -10030,7 +10030,7 @@
       <c r="AE58" s="4"/>
       <c r="AF58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
@@ -10110,7 +10110,7 @@
       <c r="AE59" s="4"/>
       <c r="AF59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
@@ -10190,7 +10190,7 @@
       <c r="AE60" s="4"/>
       <c r="AF60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>60</v>
       </c>
@@ -10270,7 +10270,7 @@
       <c r="AE61" s="4"/>
       <c r="AF61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>61</v>
       </c>
@@ -10350,7 +10350,7 @@
       <c r="AE62" s="4"/>
       <c r="AF62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
@@ -10430,7 +10430,7 @@
       <c r="AE63" s="4"/>
       <c r="AF63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
@@ -10510,7 +10510,7 @@
       <c r="AE64" s="4"/>
       <c r="AF64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <v>64</v>
       </c>
@@ -10590,7 +10590,7 @@
       <c r="AE65" s="4"/>
       <c r="AF65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <v>65</v>
       </c>
@@ -10670,7 +10670,7 @@
       <c r="AE66" s="4"/>
       <c r="AF66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>66</v>
       </c>
@@ -10750,7 +10750,7 @@
       <c r="AE67" s="4"/>
       <c r="AF67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>67</v>
       </c>
@@ -10830,7 +10830,7 @@
       <c r="AE68" s="4"/>
       <c r="AF68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <v>68</v>
       </c>
@@ -10910,7 +10910,7 @@
       <c r="AE69" s="4"/>
       <c r="AF69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <v>69</v>
       </c>
@@ -10990,7 +10990,7 @@
       <c r="AE70" s="4"/>
       <c r="AF70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <v>70</v>
       </c>
@@ -11070,7 +11070,7 @@
       <c r="AE71" s="4"/>
       <c r="AF71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <v>71</v>
       </c>
@@ -11150,7 +11150,7 @@
       <c r="AE72" s="4"/>
       <c r="AF72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
         <v>72</v>
       </c>
@@ -11230,7 +11230,7 @@
       <c r="AE73" s="4"/>
       <c r="AF73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
         <v>73</v>
       </c>
@@ -11310,7 +11310,7 @@
       <c r="AE74" s="4"/>
       <c r="AF74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <v>74</v>
       </c>
@@ -11390,7 +11390,7 @@
       <c r="AE75" s="4"/>
       <c r="AF75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
         <v>75</v>
       </c>
@@ -11470,7 +11470,7 @@
       <c r="AE76" s="4"/>
       <c r="AF76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <v>76</v>
       </c>
@@ -11550,7 +11550,7 @@
       <c r="AE77" s="4"/>
       <c r="AF77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
         <v>77</v>
       </c>
@@ -11630,7 +11630,7 @@
       <c r="AE78" s="4"/>
       <c r="AF78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
         <v>78</v>
       </c>
@@ -11710,7 +11710,7 @@
       <c r="AE79" s="4"/>
       <c r="AF79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
         <v>79</v>
       </c>
@@ -11790,7 +11790,7 @@
       <c r="AE80" s="4"/>
       <c r="AF80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
         <v>80</v>
       </c>
@@ -11870,7 +11870,7 @@
       <c r="AE81" s="4"/>
       <c r="AF81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
         <v>81</v>
       </c>
@@ -11950,7 +11950,7 @@
       <c r="AE82" s="4"/>
       <c r="AF82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
         <v>82</v>
       </c>
@@ -12030,7 +12030,7 @@
       <c r="AE83" s="4"/>
       <c r="AF83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
         <v>83</v>
       </c>
@@ -12110,7 +12110,7 @@
       <c r="AE84" s="4"/>
       <c r="AF84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
         <v>84</v>
       </c>
@@ -12190,7 +12190,7 @@
       <c r="AE85" s="4"/>
       <c r="AF85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
         <v>85</v>
       </c>
@@ -12270,7 +12270,7 @@
       <c r="AE86" s="4"/>
       <c r="AF86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
         <v>86</v>
       </c>
@@ -12350,7 +12350,7 @@
       <c r="AE87" s="4"/>
       <c r="AF87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
         <v>87</v>
       </c>
@@ -12430,7 +12430,7 @@
       <c r="AE88" s="4"/>
       <c r="AF88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
         <v>88</v>
       </c>
@@ -12510,7 +12510,7 @@
       <c r="AE89" s="4"/>
       <c r="AF89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
         <v>89</v>
       </c>
@@ -12590,7 +12590,7 @@
       <c r="AE90" s="4"/>
       <c r="AF90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
         <v>90</v>
       </c>
@@ -12670,7 +12670,7 @@
       <c r="AE91" s="4"/>
       <c r="AF91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
         <v>91</v>
       </c>
@@ -12750,7 +12750,7 @@
       <c r="AE92" s="4"/>
       <c r="AF92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
         <v>92</v>
       </c>
@@ -12830,7 +12830,7 @@
       <c r="AE93" s="4"/>
       <c r="AF93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
         <v>93</v>
       </c>
@@ -12910,7 +12910,7 @@
       <c r="AE94" s="4"/>
       <c r="AF94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
         <v>94</v>
       </c>
@@ -12990,7 +12990,7 @@
       <c r="AE95" s="4"/>
       <c r="AF95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
         <v>95</v>
       </c>
@@ -13070,7 +13070,7 @@
       <c r="AE96" s="4"/>
       <c r="AF96" s="4"/>
     </row>
-    <row r="97" customFormat="false" ht="28.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="28.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
         <v>96</v>
       </c>
@@ -13148,7 +13148,7 @@
       <c r="AE97" s="4"/>
       <c r="AF97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
         <v>97</v>
       </c>
@@ -13228,7 +13228,7 @@
       <c r="AE98" s="4"/>
       <c r="AF98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
         <v>98</v>
       </c>
@@ -13308,7 +13308,7 @@
       <c r="AE99" s="4"/>
       <c r="AF99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
         <v>99</v>
       </c>
@@ -13388,7 +13388,7 @@
       <c r="AE100" s="4"/>
       <c r="AF100" s="4"/>
     </row>
-    <row r="101" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
         <v>100</v>
       </c>
@@ -13468,7 +13468,7 @@
       <c r="AE101" s="4"/>
       <c r="AF101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
         <v>101</v>
       </c>
@@ -13548,7 +13548,7 @@
       <c r="AE102" s="4"/>
       <c r="AF102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="n">
         <v>102</v>
       </c>
@@ -13628,7 +13628,7 @@
       <c r="AE103" s="4"/>
       <c r="AF103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="n">
         <v>103</v>
       </c>
@@ -13708,12 +13708,12 @@
       <c r="AE104" s="4"/>
       <c r="AF104" s="4"/>
     </row>
-    <row r="105" customFormat="false" ht="171.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
         <v>269</v>
       </c>
       <c r="B105" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>432</v>
@@ -13788,12 +13788,12 @@
       <c r="AE105" s="4"/>
       <c r="AF105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="199.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
         <v>270</v>
       </c>
       <c r="B106" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>432</v>
@@ -13868,12 +13868,12 @@
       <c r="AE106" s="4"/>
       <c r="AF106" s="4"/>
     </row>
-    <row r="107" customFormat="false" ht="185.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="184.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="n">
         <v>271</v>
       </c>
       <c r="B107" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>432</v>
@@ -13948,12 +13948,12 @@
       <c r="AE107" s="4"/>
       <c r="AF107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="171.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
         <v>272</v>
       </c>
       <c r="B108" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>432</v>
@@ -14028,12 +14028,12 @@
       <c r="AE108" s="4"/>
       <c r="AF108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="256.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="254.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
         <v>273</v>
       </c>
       <c r="B109" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>432</v>
@@ -14108,12 +14108,12 @@
       <c r="AE109" s="4"/>
       <c r="AF109" s="4"/>
     </row>
-    <row r="110" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="n">
         <v>274</v>
       </c>
       <c r="B110" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>432</v>
@@ -14188,12 +14188,12 @@
       <c r="AE110" s="4"/>
       <c r="AF110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
         <v>275</v>
       </c>
       <c r="B111" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>432</v>
@@ -14268,12 +14268,12 @@
       <c r="AE111" s="4"/>
       <c r="AF111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="n">
         <v>276</v>
       </c>
       <c r="B112" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>432</v>
@@ -14348,12 +14348,12 @@
       <c r="AE112" s="4"/>
       <c r="AF112" s="4"/>
     </row>
-    <row r="113" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
         <v>277</v>
       </c>
       <c r="B113" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>432</v>
@@ -14428,12 +14428,12 @@
       <c r="AE113" s="4"/>
       <c r="AF113" s="4"/>
     </row>
-    <row r="114" customFormat="false" ht="114.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
         <v>278</v>
       </c>
       <c r="B114" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>432</v>
@@ -14508,12 +14508,12 @@
       <c r="AE114" s="4"/>
       <c r="AF114" s="4"/>
     </row>
-    <row r="115" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
         <v>279</v>
       </c>
       <c r="B115" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>432</v>
@@ -14586,12 +14586,12 @@
       <c r="AE115" s="4"/>
       <c r="AF115" s="4"/>
     </row>
-    <row r="116" customFormat="false" ht="184.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="184.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
         <v>280</v>
       </c>
       <c r="B116" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>432</v>
@@ -14664,12 +14664,12 @@
       <c r="AE116" s="4"/>
       <c r="AF116" s="4"/>
     </row>
-    <row r="117" customFormat="false" ht="254.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="254.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
         <v>281</v>
       </c>
       <c r="B117" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>432</v>
@@ -14742,12 +14742,12 @@
       <c r="AE117" s="4"/>
       <c r="AF117" s="4"/>
     </row>
-    <row r="118" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
         <v>282</v>
       </c>
       <c r="B118" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>432</v>
@@ -14820,12 +14820,12 @@
       <c r="AE118" s="4"/>
       <c r="AF118" s="4"/>
     </row>
-    <row r="119" customFormat="false" ht="270.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="269.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
         <v>283</v>
       </c>
       <c r="B119" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>432</v>
@@ -14898,12 +14898,12 @@
       <c r="AE119" s="4"/>
       <c r="AF119" s="4"/>
     </row>
-    <row r="120" customFormat="false" ht="228.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
         <v>284</v>
       </c>
       <c r="B120" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>432</v>
@@ -14976,12 +14976,12 @@
       <c r="AE120" s="4"/>
       <c r="AF120" s="4"/>
     </row>
-    <row r="121" customFormat="false" ht="228.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
         <v>285</v>
       </c>
       <c r="B121" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>432</v>
@@ -15054,12 +15054,12 @@
       <c r="AE121" s="4"/>
       <c r="AF121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="242.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="241.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
         <v>286</v>
       </c>
       <c r="B122" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>432</v>
@@ -15132,12 +15132,12 @@
       <c r="AE122" s="4"/>
       <c r="AF122" s="4"/>
     </row>
-    <row r="123" customFormat="false" ht="214.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="212.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
         <v>287</v>
       </c>
       <c r="B123" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>432</v>
@@ -15210,12 +15210,12 @@
       <c r="AE123" s="4"/>
       <c r="AF123" s="4"/>
     </row>
-    <row r="124" customFormat="false" ht="228.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
         <v>288</v>
       </c>
       <c r="B124" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>432</v>
@@ -15288,12 +15288,12 @@
       <c r="AE124" s="4"/>
       <c r="AF124" s="4"/>
     </row>
-    <row r="125" customFormat="false" ht="299.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
         <v>289</v>
       </c>
       <c r="B125" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>432</v>
@@ -15368,12 +15368,12 @@
       <c r="AE125" s="4"/>
       <c r="AF125" s="4"/>
     </row>
-    <row r="126" customFormat="false" ht="184.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="184.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
         <v>290</v>
       </c>
       <c r="B126" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>432</v>
@@ -15448,12 +15448,12 @@
       <c r="AE126" s="4"/>
       <c r="AF126" s="4"/>
     </row>
-    <row r="127" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="n">
         <v>291</v>
       </c>
       <c r="B127" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>432</v>
@@ -15528,12 +15528,12 @@
       <c r="AE127" s="4"/>
       <c r="AF127" s="4"/>
     </row>
-    <row r="128" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="n">
         <v>292</v>
       </c>
       <c r="B128" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>432</v>
@@ -15608,12 +15608,12 @@
       <c r="AE128" s="4"/>
       <c r="AF128" s="4"/>
     </row>
-    <row r="129" customFormat="false" ht="212.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="212.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="n">
         <v>293</v>
       </c>
       <c r="B129" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>432</v>
@@ -15688,12 +15688,12 @@
       <c r="AE129" s="4"/>
       <c r="AF129" s="4"/>
     </row>
-    <row r="130" customFormat="false" ht="285.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
         <v>294</v>
       </c>
       <c r="B130" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>432</v>
@@ -15768,12 +15768,12 @@
       <c r="AE130" s="4"/>
       <c r="AF130" s="4"/>
     </row>
-    <row r="131" customFormat="false" ht="270.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="269.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="n">
         <v>295</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>432</v>
@@ -15848,12 +15848,12 @@
       <c r="AE131" s="4"/>
       <c r="AF131" s="4"/>
     </row>
-    <row r="132" customFormat="false" ht="228.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
         <v>296</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>432</v>
@@ -15928,12 +15928,12 @@
       <c r="AE132" s="4"/>
       <c r="AF132" s="4"/>
     </row>
-    <row r="133" customFormat="false" ht="228.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="n">
         <v>297</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>432</v>
@@ -16008,12 +16008,12 @@
       <c r="AE133" s="4"/>
       <c r="AF133" s="4"/>
     </row>
-    <row r="134" customFormat="false" ht="114.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
         <v>298</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>432</v>
@@ -16086,12 +16086,12 @@
       <c r="AE134" s="4"/>
       <c r="AF134" s="4"/>
     </row>
-    <row r="135" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="n">
         <v>299</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>432</v>
@@ -16166,12 +16166,12 @@
       <c r="AE135" s="4"/>
       <c r="AF135" s="4"/>
     </row>
-    <row r="136" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="n">
         <v>300</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>432</v>
@@ -16246,12 +16246,12 @@
       <c r="AE136" s="4"/>
       <c r="AF136" s="4"/>
     </row>
-    <row r="137" customFormat="false" ht="269.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="269.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
         <v>301</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>432</v>
@@ -16326,12 +16326,12 @@
       <c r="AE137" s="4"/>
       <c r="AF137" s="4"/>
     </row>
-    <row r="138" customFormat="false" ht="212.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="212.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
         <v>302</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>432</v>
@@ -16406,12 +16406,12 @@
       <c r="AE138" s="4"/>
       <c r="AF138" s="4"/>
     </row>
-    <row r="139" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="n">
         <v>303</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>432</v>
@@ -16486,12 +16486,12 @@
       <c r="AE139" s="4"/>
       <c r="AF139" s="4"/>
     </row>
-    <row r="140" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
         <v>304</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>432</v>
@@ -16566,12 +16566,12 @@
       <c r="AE140" s="4"/>
       <c r="AF140" s="4"/>
     </row>
-    <row r="141" customFormat="false" ht="283.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
         <v>305</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>432</v>
@@ -16646,12 +16646,12 @@
       <c r="AE141" s="4"/>
       <c r="AF141" s="4"/>
     </row>
-    <row r="142" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
         <v>306</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>432</v>
@@ -16726,12 +16726,12 @@
       <c r="AE142" s="4"/>
       <c r="AF142" s="4"/>
     </row>
-    <row r="143" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
         <v>307</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>432</v>
@@ -16806,12 +16806,12 @@
       <c r="AE143" s="4"/>
       <c r="AF143" s="4"/>
     </row>
-    <row r="144" customFormat="false" ht="254.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="254.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
         <v>308</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>432</v>
@@ -16886,12 +16886,12 @@
       <c r="AE144" s="4"/>
       <c r="AF144" s="4"/>
     </row>
-    <row r="145" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
         <v>309</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>432</v>
@@ -16966,12 +16966,12 @@
       <c r="AE145" s="4"/>
       <c r="AF145" s="4"/>
     </row>
-    <row r="146" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="n">
         <v>310</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>432</v>
@@ -17046,12 +17046,12 @@
       <c r="AE146" s="4"/>
       <c r="AF146" s="4"/>
     </row>
-    <row r="147" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
         <v>311</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>432</v>
@@ -17126,12 +17126,12 @@
       <c r="AE147" s="4"/>
       <c r="AF147" s="4"/>
     </row>
-    <row r="148" customFormat="false" ht="269.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="269.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="n">
         <v>312</v>
       </c>
       <c r="B148" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>432</v>
@@ -17206,12 +17206,12 @@
       <c r="AE148" s="4"/>
       <c r="AF148" s="4"/>
     </row>
-    <row r="149" customFormat="false" ht="157.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="n">
         <v>313</v>
       </c>
       <c r="B149" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>432</v>
@@ -17286,12 +17286,12 @@
       <c r="AE149" s="4"/>
       <c r="AF149" s="4"/>
     </row>
-    <row r="150" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="n">
         <v>314</v>
       </c>
       <c r="B150" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>432</v>
@@ -17366,12 +17366,12 @@
       <c r="AE150" s="4"/>
       <c r="AF150" s="4"/>
     </row>
-    <row r="151" customFormat="false" ht="184.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="184.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="n">
         <v>315</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>432</v>
@@ -17446,12 +17446,12 @@
       <c r="AE151" s="4"/>
       <c r="AF151" s="4"/>
     </row>
-    <row r="152" customFormat="false" ht="212.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="212.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
         <v>316</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>432</v>
@@ -17526,12 +17526,12 @@
       <c r="AE152" s="4"/>
       <c r="AF152" s="4"/>
     </row>
-    <row r="153" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
         <v>317</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>432</v>
@@ -17606,12 +17606,12 @@
       <c r="AE153" s="4"/>
       <c r="AF153" s="4"/>
     </row>
-    <row r="154" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
         <v>318</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>432</v>
@@ -17684,12 +17684,12 @@
       <c r="AE154" s="4"/>
       <c r="AF154" s="4"/>
     </row>
-    <row r="155" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
         <v>319</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>432</v>
@@ -17762,12 +17762,12 @@
       <c r="AE155" s="4"/>
       <c r="AF155" s="4"/>
     </row>
-    <row r="156" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
         <v>320</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>432</v>
@@ -17840,12 +17840,12 @@
       <c r="AE156" s="4"/>
       <c r="AF156" s="4"/>
     </row>
-    <row r="157" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
         <v>321</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>432</v>
@@ -17918,12 +17918,12 @@
       <c r="AE157" s="4"/>
       <c r="AF157" s="4"/>
     </row>
-    <row r="158" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
         <v>322</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>432</v>
@@ -17996,12 +17996,12 @@
       <c r="AE158" s="4"/>
       <c r="AF158" s="4"/>
     </row>
-    <row r="159" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="n">
         <v>323</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>432</v>
@@ -18074,12 +18074,12 @@
       <c r="AE159" s="4"/>
       <c r="AF159" s="4"/>
     </row>
-    <row r="160" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
         <v>324</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>432</v>
@@ -18154,12 +18154,12 @@
       <c r="AE160" s="4"/>
       <c r="AF160" s="4"/>
     </row>
-    <row r="161" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="n">
         <v>325</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>432</v>
@@ -18234,12 +18234,12 @@
       <c r="AE161" s="4"/>
       <c r="AF161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="184.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="184.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
         <v>326</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>432</v>
@@ -18314,12 +18314,12 @@
       <c r="AE162" s="4"/>
       <c r="AF162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="241.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="241.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
         <v>327</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>432</v>
@@ -18392,12 +18392,12 @@
       <c r="AE163" s="4"/>
       <c r="AF163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
         <v>328</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>432</v>
@@ -18472,12 +18472,12 @@
       <c r="AE164" s="4"/>
       <c r="AF164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
         <v>329</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>432</v>
@@ -18552,12 +18552,12 @@
       <c r="AE165" s="4"/>
       <c r="AF165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
         <v>330</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>432</v>
@@ -18630,12 +18630,12 @@
       <c r="AE166" s="4"/>
       <c r="AF166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
         <v>331</v>
       </c>
       <c r="B167" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>432</v>
@@ -18710,12 +18710,12 @@
       <c r="AE167" s="4"/>
       <c r="AF167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
         <v>332</v>
       </c>
       <c r="B168" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>432</v>
@@ -18790,12 +18790,12 @@
       <c r="AE168" s="4"/>
       <c r="AF168" s="4"/>
     </row>
-    <row r="169" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
         <v>333</v>
       </c>
       <c r="B169" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>432</v>
@@ -18870,12 +18870,12 @@
       <c r="AE169" s="4"/>
       <c r="AF169" s="4"/>
     </row>
-    <row r="170" customFormat="false" ht="171.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
         <v>334</v>
       </c>
       <c r="B170" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>432</v>
@@ -18950,12 +18950,12 @@
       </c>
       <c r="AF170" s="4"/>
     </row>
-    <row r="171" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
         <v>335</v>
       </c>
       <c r="B171" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>432</v>
@@ -19030,12 +19030,12 @@
       </c>
       <c r="AF171" s="4"/>
     </row>
-    <row r="172" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
         <v>336</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>432</v>
@@ -19110,12 +19110,12 @@
       </c>
       <c r="AF172" s="4"/>
     </row>
-    <row r="173" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
         <v>337</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>432</v>
@@ -19190,12 +19190,12 @@
       </c>
       <c r="AF173" s="4"/>
     </row>
-    <row r="174" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
         <v>338</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>432</v>
@@ -19270,12 +19270,12 @@
       </c>
       <c r="AF174" s="4"/>
     </row>
-    <row r="175" customFormat="false" ht="129.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="n">
         <v>339</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>432</v>
@@ -19350,12 +19350,12 @@
       </c>
       <c r="AF175" s="4"/>
     </row>
-    <row r="176" customFormat="false" ht="157.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="n">
         <v>340</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>432</v>
@@ -19430,12 +19430,12 @@
       </c>
       <c r="AF176" s="4"/>
     </row>
-    <row r="177" customFormat="false" ht="157.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="n">
         <v>341</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>432</v>
@@ -19510,12 +19510,12 @@
       </c>
       <c r="AF177" s="4"/>
     </row>
-    <row r="178" customFormat="false" ht="157.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="n">
         <v>342</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>432</v>
@@ -19590,12 +19590,12 @@
       </c>
       <c r="AF178" s="4"/>
     </row>
-    <row r="179" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
         <v>343</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>432</v>
@@ -19670,12 +19670,12 @@
       </c>
       <c r="AF179" s="4"/>
     </row>
-    <row r="180" customFormat="false" ht="212.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="212.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
         <v>344</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>432</v>
@@ -19750,12 +19750,12 @@
       </c>
       <c r="AF180" s="4"/>
     </row>
-    <row r="181" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="n">
         <v>345</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>432</v>
@@ -19832,12 +19832,12 @@
       </c>
       <c r="AF181" s="4"/>
     </row>
-    <row r="182" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="n">
         <v>346</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>432</v>
@@ -19914,12 +19914,12 @@
       </c>
       <c r="AF182" s="4"/>
     </row>
-    <row r="183" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="n">
         <v>347</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>432</v>
@@ -19996,12 +19996,12 @@
       </c>
       <c r="AF183" s="4"/>
     </row>
-    <row r="184" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="n">
         <v>348</v>
       </c>
       <c r="B184" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>432</v>
@@ -20076,12 +20076,12 @@
       </c>
       <c r="AF184" s="4"/>
     </row>
-    <row r="185" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
         <v>349</v>
       </c>
       <c r="B185" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>432</v>
@@ -20156,12 +20156,12 @@
       </c>
       <c r="AF185" s="4"/>
     </row>
-    <row r="186" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
         <v>350</v>
       </c>
       <c r="B186" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>432</v>
@@ -20236,12 +20236,12 @@
       </c>
       <c r="AF186" s="4"/>
     </row>
-    <row r="187" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
         <v>351</v>
       </c>
       <c r="B187" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>432</v>
@@ -20316,12 +20316,12 @@
       </c>
       <c r="AF187" s="4"/>
     </row>
-    <row r="188" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
         <v>352</v>
       </c>
       <c r="B188" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>432</v>
@@ -20396,12 +20396,12 @@
       </c>
       <c r="AF188" s="4"/>
     </row>
-    <row r="189" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
         <v>353</v>
       </c>
       <c r="B189" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>432</v>
@@ -20476,12 +20476,12 @@
       </c>
       <c r="AF189" s="4"/>
     </row>
-    <row r="190" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
         <v>354</v>
       </c>
       <c r="B190" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>432</v>
@@ -20556,12 +20556,12 @@
       </c>
       <c r="AF190" s="4"/>
     </row>
-    <row r="191" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
         <v>355</v>
       </c>
       <c r="B191" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>432</v>
@@ -20636,12 +20636,12 @@
       </c>
       <c r="AF191" s="4"/>
     </row>
-    <row r="192" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
         <v>356</v>
       </c>
       <c r="B192" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>432</v>
@@ -20716,12 +20716,12 @@
       </c>
       <c r="AF192" s="4"/>
     </row>
-    <row r="193" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="n">
         <v>357</v>
       </c>
       <c r="B193" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>432</v>
@@ -20796,12 +20796,12 @@
       </c>
       <c r="AF193" s="4"/>
     </row>
-    <row r="194" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
         <v>358</v>
       </c>
       <c r="B194" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>432</v>
@@ -20876,12 +20876,12 @@
       </c>
       <c r="AF194" s="4"/>
     </row>
-    <row r="195" customFormat="false" ht="227.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="227.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
         <v>359</v>
       </c>
       <c r="B195" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>432</v>
@@ -20956,12 +20956,12 @@
       </c>
       <c r="AF195" s="4"/>
     </row>
-    <row r="196" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
         <v>360</v>
       </c>
       <c r="B196" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>432</v>
@@ -21036,12 +21036,12 @@
       </c>
       <c r="AF196" s="4"/>
     </row>
-    <row r="197" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
         <v>361</v>
       </c>
       <c r="B197" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>432</v>
@@ -21116,12 +21116,12 @@
       </c>
       <c r="AF197" s="4"/>
     </row>
-    <row r="198" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="n">
         <v>362</v>
       </c>
       <c r="B198" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>432</v>
@@ -21196,12 +21196,12 @@
       </c>
       <c r="AF198" s="4"/>
     </row>
-    <row r="199" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
         <v>363</v>
       </c>
       <c r="B199" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>432</v>
@@ -21276,12 +21276,12 @@
       </c>
       <c r="AF199" s="4"/>
     </row>
-    <row r="200" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="n">
         <v>364</v>
       </c>
       <c r="B200" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>432</v>
@@ -21356,12 +21356,12 @@
       </c>
       <c r="AF200" s="4"/>
     </row>
-    <row r="201" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="n">
         <v>365</v>
       </c>
       <c r="B201" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>432</v>
@@ -21436,12 +21436,12 @@
       </c>
       <c r="AF201" s="4"/>
     </row>
-    <row r="202" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
         <v>366</v>
       </c>
       <c r="B202" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>432</v>
@@ -21516,12 +21516,12 @@
       </c>
       <c r="AF202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="n">
         <v>367</v>
       </c>
       <c r="B203" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>432</v>
@@ -21596,12 +21596,12 @@
       </c>
       <c r="AF203" s="4"/>
     </row>
-    <row r="204" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
         <v>368</v>
       </c>
       <c r="B204" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>432</v>
@@ -21676,12 +21676,12 @@
       </c>
       <c r="AF204" s="4"/>
     </row>
-    <row r="205" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
         <v>369</v>
       </c>
       <c r="B205" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>432</v>
@@ -21756,12 +21756,12 @@
       </c>
       <c r="AF205" s="4"/>
     </row>
-    <row r="206" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
         <v>370</v>
       </c>
       <c r="B206" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>432</v>
@@ -21836,12 +21836,12 @@
       </c>
       <c r="AF206" s="4"/>
     </row>
-    <row r="207" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
         <v>371</v>
       </c>
       <c r="B207" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>432</v>
@@ -21916,12 +21916,12 @@
       </c>
       <c r="AF207" s="4"/>
     </row>
-    <row r="208" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="n">
         <v>372</v>
       </c>
       <c r="B208" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>432</v>
@@ -21996,12 +21996,12 @@
       </c>
       <c r="AF208" s="4"/>
     </row>
-    <row r="209" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="n">
         <v>373</v>
       </c>
       <c r="B209" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>432</v>
@@ -22076,12 +22076,12 @@
       </c>
       <c r="AF209" s="4"/>
     </row>
-    <row r="210" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="n">
         <v>374</v>
       </c>
       <c r="B210" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>432</v>
@@ -22156,12 +22156,12 @@
       </c>
       <c r="AF210" s="4"/>
     </row>
-    <row r="211" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="n">
         <v>375</v>
       </c>
       <c r="B211" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>432</v>
@@ -22236,12 +22236,12 @@
       </c>
       <c r="AF211" s="4"/>
     </row>
-    <row r="212" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="n">
         <v>376</v>
       </c>
       <c r="B212" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>432</v>
@@ -22316,12 +22316,12 @@
       </c>
       <c r="AF212" s="4"/>
     </row>
-    <row r="213" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="n">
         <v>377</v>
       </c>
       <c r="B213" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>432</v>
@@ -22396,12 +22396,12 @@
       </c>
       <c r="AF213" s="4"/>
     </row>
-    <row r="214" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="n">
         <v>378</v>
       </c>
       <c r="B214" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>432</v>
@@ -22476,12 +22476,12 @@
       </c>
       <c r="AF214" s="4"/>
     </row>
-    <row r="215" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="n">
         <v>379</v>
       </c>
       <c r="B215" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>432</v>
@@ -22556,12 +22556,12 @@
       </c>
       <c r="AF215" s="4"/>
     </row>
-    <row r="216" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="n">
         <v>380</v>
       </c>
       <c r="B216" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>432</v>
@@ -22636,12 +22636,12 @@
       </c>
       <c r="AF216" s="4"/>
     </row>
-    <row r="217" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="n">
         <v>381</v>
       </c>
       <c r="B217" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>432</v>
@@ -22716,12 +22716,12 @@
       </c>
       <c r="AF217" s="4"/>
     </row>
-    <row r="218" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="n">
         <v>382</v>
       </c>
       <c r="B218" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>432</v>
@@ -22796,12 +22796,12 @@
       </c>
       <c r="AF218" s="4"/>
     </row>
-    <row r="219" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="n">
         <v>383</v>
       </c>
       <c r="B219" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>432</v>
@@ -22876,12 +22876,12 @@
       </c>
       <c r="AF219" s="4"/>
     </row>
-    <row r="220" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="n">
         <v>384</v>
       </c>
       <c r="B220" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>432</v>
@@ -22956,12 +22956,12 @@
       </c>
       <c r="AF220" s="4"/>
     </row>
-    <row r="221" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="n">
         <v>385</v>
       </c>
       <c r="B221" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>432</v>
@@ -23036,12 +23036,12 @@
       </c>
       <c r="AF221" s="4"/>
     </row>
-    <row r="222" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="n">
         <v>386</v>
       </c>
       <c r="B222" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C222" s="4" t="s">
         <v>432</v>
@@ -23116,12 +23116,12 @@
       </c>
       <c r="AF222" s="4"/>
     </row>
-    <row r="223" customFormat="false" ht="198.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="198.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="n">
         <v>387</v>
       </c>
       <c r="B223" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>432</v>
@@ -23196,12 +23196,12 @@
       </c>
       <c r="AF223" s="4"/>
     </row>
-    <row r="224" customFormat="false" ht="156.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="156.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="n">
         <v>388</v>
       </c>
       <c r="B224" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>432</v>
@@ -23276,12 +23276,12 @@
       </c>
       <c r="AF224" s="4"/>
     </row>
-    <row r="225" customFormat="false" ht="86.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="n">
         <v>389</v>
       </c>
       <c r="B225" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>432</v>
@@ -23356,12 +23356,12 @@
       </c>
       <c r="AF225" s="4"/>
     </row>
-    <row r="226" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="n">
         <v>390</v>
       </c>
       <c r="B226" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>432</v>
@@ -23436,12 +23436,12 @@
       </c>
       <c r="AF226" s="4"/>
     </row>
-    <row r="227" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
         <v>391</v>
       </c>
       <c r="B227" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>432</v>
@@ -23516,12 +23516,12 @@
       </c>
       <c r="AF227" s="4"/>
     </row>
-    <row r="228" customFormat="false" ht="142.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="142.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="n">
         <v>392</v>
       </c>
       <c r="B228" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>432</v>
@@ -23596,12 +23596,12 @@
       </c>
       <c r="AF228" s="4"/>
     </row>
-    <row r="229" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="n">
         <v>393</v>
       </c>
       <c r="B229" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>432</v>
@@ -23676,12 +23676,12 @@
       </c>
       <c r="AF229" s="4"/>
     </row>
-    <row r="230" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="n">
         <v>394</v>
       </c>
       <c r="B230" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>432</v>
@@ -23756,12 +23756,12 @@
       </c>
       <c r="AF230" s="4"/>
     </row>
-    <row r="231" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="n">
         <v>395</v>
       </c>
       <c r="B231" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>432</v>
@@ -23836,12 +23836,12 @@
       </c>
       <c r="AF231" s="4"/>
     </row>
-    <row r="232" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
         <v>396</v>
       </c>
       <c r="B232" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>432</v>
@@ -23916,12 +23916,12 @@
       </c>
       <c r="AF232" s="4"/>
     </row>
-    <row r="233" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
         <v>397</v>
       </c>
       <c r="B233" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>432</v>
@@ -23996,12 +23996,12 @@
       </c>
       <c r="AF233" s="4"/>
     </row>
-    <row r="234" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="n">
         <v>398</v>
       </c>
       <c r="B234" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>432</v>
@@ -24076,12 +24076,12 @@
       </c>
       <c r="AF234" s="4"/>
     </row>
-    <row r="235" customFormat="false" ht="42.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="42.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="n">
         <v>399</v>
       </c>
       <c r="B235" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>432</v>
@@ -24156,12 +24156,12 @@
       </c>
       <c r="AF235" s="4"/>
     </row>
-    <row r="236" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
         <v>400</v>
       </c>
       <c r="B236" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>432</v>
@@ -24236,12 +24236,12 @@
       </c>
       <c r="AF236" s="4"/>
     </row>
-    <row r="237" customFormat="false" ht="28.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="28.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="n">
         <v>401</v>
       </c>
       <c r="B237" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>432</v>
@@ -24314,12 +24314,12 @@
       </c>
       <c r="AF237" s="4"/>
     </row>
-    <row r="238" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="n">
         <v>402</v>
       </c>
       <c r="B238" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>432</v>
@@ -24394,12 +24394,12 @@
       </c>
       <c r="AF238" s="4"/>
     </row>
-    <row r="239" customFormat="false" ht="113.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="113.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="n">
         <v>403</v>
       </c>
       <c r="B239" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>432</v>
@@ -24474,12 +24474,12 @@
       </c>
       <c r="AF239" s="4"/>
     </row>
-    <row r="240" customFormat="false" ht="169.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="169.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="n">
         <v>404</v>
       </c>
       <c r="B240" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>432</v>
@@ -24554,12 +24554,12 @@
       </c>
       <c r="AF240" s="4"/>
     </row>
-    <row r="241" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="n">
         <v>405</v>
       </c>
       <c r="B241" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>432</v>
@@ -24634,12 +24634,12 @@
       </c>
       <c r="AF241" s="4"/>
     </row>
-    <row r="242" customFormat="false" ht="127.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="127.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="n">
         <v>406</v>
       </c>
       <c r="B242" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>432</v>
@@ -24714,12 +24714,12 @@
       </c>
       <c r="AF242" s="4"/>
     </row>
-    <row r="243" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
         <v>407</v>
       </c>
       <c r="B243" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>432</v>
@@ -24794,12 +24794,12 @@
       </c>
       <c r="AF243" s="4"/>
     </row>
-    <row r="244" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="n">
         <v>408</v>
       </c>
       <c r="B244" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>432</v>
@@ -24874,12 +24874,12 @@
       </c>
       <c r="AF244" s="4"/>
     </row>
-    <row r="245" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="n">
         <v>409</v>
       </c>
       <c r="B245" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>432</v>
@@ -24954,12 +24954,12 @@
       </c>
       <c r="AF245" s="4"/>
     </row>
-    <row r="246" customFormat="false" ht="56.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
         <v>410</v>
       </c>
       <c r="B246" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>432</v>
@@ -25034,12 +25034,12 @@
       </c>
       <c r="AF246" s="4"/>
     </row>
-    <row r="247" customFormat="false" ht="84.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="n">
         <v>411</v>
       </c>
       <c r="B247" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>432</v>
@@ -25114,12 +25114,12 @@
       </c>
       <c r="AF247" s="4"/>
     </row>
-    <row r="248" customFormat="false" ht="99.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="99.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="n">
         <v>412</v>
       </c>
       <c r="B248" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>432</v>
@@ -25194,12 +25194,12 @@
       </c>
       <c r="AF248" s="4"/>
     </row>
-    <row r="249" customFormat="false" ht="71.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="71.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="n">
         <v>413</v>
       </c>
       <c r="B249" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>432</v>
@@ -25274,12 +25274,12 @@
       </c>
       <c r="AF249" s="4"/>
     </row>
-    <row r="250" customFormat="false" ht="148.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="148.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="11" t="n">
         <v>414</v>
       </c>
       <c r="B250" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C250" s="12" t="s">
         <v>960</v>
@@ -25355,12 +25355,12 @@
         <v>969</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="11" t="n">
         <v>415</v>
       </c>
       <c r="B251" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C251" s="12" t="s">
         <v>960</v>
@@ -25434,12 +25434,12 @@
         <v>973</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="174.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="174.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="11" t="n">
         <v>416</v>
       </c>
       <c r="B252" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C252" s="12" t="s">
         <v>960</v>
@@ -25509,12 +25509,12 @@
       <c r="AD252" s="12"/>
       <c r="AE252" s="12"/>
     </row>
-    <row r="253" customFormat="false" ht="160.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="160.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="11" t="n">
         <v>417</v>
       </c>
       <c r="B253" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C253" s="12" t="s">
         <v>960</v>
@@ -25584,12 +25584,12 @@
       <c r="AD253" s="12"/>
       <c r="AE253" s="12"/>
     </row>
-    <row r="254" customFormat="false" ht="148.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="148.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="11" t="n">
         <v>418</v>
       </c>
       <c r="B254" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C254" s="12" t="s">
         <v>960</v>
@@ -25659,12 +25659,12 @@
       <c r="AD254" s="12"/>
       <c r="AE254" s="12"/>
     </row>
-    <row r="255" customFormat="false" ht="160.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="160.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="11" t="n">
         <v>419</v>
       </c>
       <c r="B255" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C255" s="12" t="s">
         <v>960</v>
@@ -25740,12 +25740,12 @@
         <v>969</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="66.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="11" t="n">
         <v>420</v>
       </c>
       <c r="B256" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C256" s="12" t="s">
         <v>960</v>
@@ -25821,12 +25821,12 @@
         <v>969</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="160.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="160.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="11" t="n">
         <v>421</v>
       </c>
       <c r="B257" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C257" s="12" t="s">
         <v>960</v>
@@ -25902,12 +25902,12 @@
         <v>996</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="160.7" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="160.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="11" t="n">
         <v>422</v>
       </c>
       <c r="B258" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C258" s="12" t="s">
         <v>960</v>
@@ -25983,12 +25983,12 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="134.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="134.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="11" t="n">
         <v>423</v>
       </c>
       <c r="B259" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C259" s="12" t="s">
         <v>960</v>
@@ -26063,7 +26063,7 @@
         <v>424</v>
       </c>
       <c r="B260" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C260" s="12" t="s">
         <v>960</v>
@@ -26140,7 +26140,7 @@
         <v>425</v>
       </c>
       <c r="B261" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C261" s="12" t="s">
         <v>960</v>
@@ -26217,7 +26217,7 @@
         <v>426</v>
       </c>
       <c r="B262" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C262" s="12" t="s">
         <v>960</v>
@@ -26294,7 +26294,7 @@
         <v>427</v>
       </c>
       <c r="B263" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C263" s="12" t="s">
         <v>960</v>
@@ -26371,7 +26371,7 @@
         <v>428</v>
       </c>
       <c r="B264" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C264" s="12" t="s">
         <v>960</v>
@@ -26448,7 +26448,7 @@
         <v>429</v>
       </c>
       <c r="B265" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C265" s="12" t="s">
         <v>960</v>
@@ -26525,7 +26525,7 @@
         <v>430</v>
       </c>
       <c r="B266" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C266" s="12" t="s">
         <v>960</v>
@@ -26602,7 +26602,7 @@
         <v>431</v>
       </c>
       <c r="B267" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C267" s="12" t="s">
         <v>960</v>
@@ -26677,7 +26677,7 @@
         <v>432</v>
       </c>
       <c r="B268" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C268" s="12" t="s">
         <v>960</v>
@@ -26752,7 +26752,7 @@
         <v>433</v>
       </c>
       <c r="B269" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C269" s="12" t="s">
         <v>960</v>
@@ -26824,12 +26824,12 @@
       <c r="AD269" s="12"/>
       <c r="AE269" s="12"/>
     </row>
-    <row r="270" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="11" t="n">
         <v>434</v>
       </c>
       <c r="B270" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C270" s="12" t="s">
         <v>960</v>
@@ -26901,12 +26901,12 @@
       <c r="AD270" s="12"/>
       <c r="AE270" s="12"/>
     </row>
-    <row r="271" customFormat="false" ht="148.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="148.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="11" t="n">
         <v>435</v>
       </c>
       <c r="B271" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C271" s="12" t="s">
         <v>960</v>
@@ -26976,12 +26976,12 @@
       <c r="AD271" s="12"/>
       <c r="AE271" s="12"/>
     </row>
-    <row r="272" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="11" t="n">
         <v>436</v>
       </c>
       <c r="B272" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C272" s="12" t="s">
         <v>960</v>
@@ -27051,12 +27051,12 @@
       <c r="AD272" s="12"/>
       <c r="AE272" s="12"/>
     </row>
-    <row r="273" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="11" t="n">
         <v>437</v>
       </c>
       <c r="B273" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C273" s="12" t="s">
         <v>960</v>
@@ -27126,12 +27126,12 @@
       <c r="AD273" s="12"/>
       <c r="AE273" s="12"/>
     </row>
-    <row r="274" customFormat="false" ht="66.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="11" t="n">
         <v>438</v>
       </c>
       <c r="B274" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C274" s="12" t="s">
         <v>960</v>
@@ -27201,12 +27201,12 @@
       <c r="AD274" s="12"/>
       <c r="AE274" s="12"/>
     </row>
-    <row r="275" customFormat="false" ht="53.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="11" t="n">
         <v>439</v>
       </c>
       <c r="B275" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C275" s="12" t="s">
         <v>960</v>
@@ -27276,12 +27276,12 @@
       <c r="AD275" s="12"/>
       <c r="AE275" s="12"/>
     </row>
-    <row r="276" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="11" t="n">
         <v>440</v>
       </c>
       <c r="B276" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C276" s="12" t="s">
         <v>960</v>
@@ -27349,12 +27349,12 @@
       <c r="AD276" s="12"/>
       <c r="AE276" s="12"/>
     </row>
-    <row r="277" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="11" t="n">
         <v>441</v>
       </c>
       <c r="B277" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C277" s="12" t="s">
         <v>960</v>
@@ -27422,12 +27422,12 @@
       <c r="AD277" s="12"/>
       <c r="AE277" s="12"/>
     </row>
-    <row r="278" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="11" t="n">
         <v>442</v>
       </c>
       <c r="B278" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C278" s="12" t="s">
         <v>960</v>
@@ -27495,12 +27495,12 @@
       <c r="AD278" s="12"/>
       <c r="AE278" s="12"/>
     </row>
-    <row r="279" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="11" t="n">
         <v>443</v>
       </c>
       <c r="B279" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C279" s="12" t="s">
         <v>960</v>
@@ -27572,12 +27572,12 @@
         <v>763</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="11" t="n">
         <v>444</v>
       </c>
       <c r="B280" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C280" s="12" t="s">
         <v>960</v>
@@ -27649,12 +27649,12 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="11" t="n">
         <v>445</v>
       </c>
       <c r="B281" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C281" s="12" t="s">
         <v>960</v>
@@ -27726,12 +27726,12 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="11" t="n">
         <v>446</v>
       </c>
       <c r="B282" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C282" s="12" t="s">
         <v>960</v>
@@ -27803,12 +27803,12 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="11" t="n">
         <v>447</v>
       </c>
       <c r="B283" s="11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C283" s="12" t="s">
         <v>960</v>
@@ -27876,7 +27876,7 @@
       <c r="AD283" s="12"/>
       <c r="AE283" s="12"/>
     </row>
-    <row r="284" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="11" t="n">
         <v>448</v>
       </c>
@@ -27953,7 +27953,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="11" t="n">
         <v>449</v>
       </c>
@@ -28030,7 +28030,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="11" t="n">
         <v>450</v>
       </c>
@@ -28107,7 +28107,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="11" t="n">
         <v>451</v>
       </c>
@@ -28184,7 +28184,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="26.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="11" t="n">
         <v>452</v>
       </c>
@@ -28261,7 +28261,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="282.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="282.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="11" t="n">
         <v>453</v>
       </c>
@@ -28336,7 +28336,7 @@
       <c r="AD289" s="12"/>
       <c r="AE289" s="12"/>
     </row>
-    <row r="290" customFormat="false" ht="120.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="120.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="11" t="n">
         <v>454</v>
       </c>
@@ -28411,7 +28411,7 @@
       <c r="AD290" s="12"/>
       <c r="AE290" s="12"/>
     </row>
-    <row r="291" customFormat="false" ht="134.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="134.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="11" t="n">
         <v>455</v>
       </c>
@@ -28486,7 +28486,7 @@
       <c r="AD291" s="12"/>
       <c r="AE291" s="12"/>
     </row>
-    <row r="292" customFormat="false" ht="174.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="174.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="11" t="n">
         <v>456</v>
       </c>
@@ -28561,7 +28561,7 @@
       <c r="AD292" s="12"/>
       <c r="AE292" s="12"/>
     </row>
-    <row r="293" customFormat="false" ht="107.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="107.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="11" t="n">
         <v>457</v>
       </c>
@@ -28636,7 +28636,7 @@
       <c r="AD293" s="12"/>
       <c r="AE293" s="12"/>
     </row>
-    <row r="294" customFormat="false" ht="40.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="11" t="n">
         <v>458</v>
       </c>
@@ -28713,7 +28713,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="40.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="11" t="n">
         <v>459</v>
       </c>
@@ -28790,7 +28790,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="66.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="11" t="n">
         <v>460</v>
       </c>
@@ -28867,7 +28867,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="40.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="11" t="n">
         <v>461</v>
       </c>
@@ -28944,7 +28944,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="40.15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="11" t="n">
         <v>462</v>
       </c>
@@ -29021,7 +29021,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="148.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="148.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="11" t="n">
         <v>463</v>
       </c>
@@ -29100,7 +29100,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="120.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="120.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="11" t="n">
         <v>464</v>
       </c>
@@ -29179,7 +29179,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="80.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="11" t="n">
         <v>465</v>
       </c>
@@ -29258,7 +29258,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="107.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="107.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="11" t="n">
         <v>466</v>
       </c>
@@ -29337,7 +29337,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="134.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="134.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="11" t="n">
         <v>467</v>
       </c>
@@ -29416,7 +29416,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="11" t="n">
         <v>468</v>
       </c>
@@ -29491,7 +29491,7 @@
       <c r="AD304" s="12"/>
       <c r="AE304" s="12"/>
     </row>
-    <row r="305" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="11" t="n">
         <v>469</v>
       </c>
@@ -29566,7 +29566,7 @@
       <c r="AD305" s="12"/>
       <c r="AE305" s="12"/>
     </row>
-    <row r="306" customFormat="false" ht="80.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="11" t="n">
         <v>470</v>
       </c>
@@ -29641,7 +29641,7 @@
       <c r="AD306" s="12"/>
       <c r="AE306" s="12"/>
     </row>
-    <row r="307" customFormat="false" ht="148.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="148.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="11" t="n">
         <v>471</v>
       </c>
@@ -29716,7 +29716,7 @@
       <c r="AD307" s="12"/>
       <c r="AE307" s="12"/>
     </row>
-    <row r="308" customFormat="false" ht="134.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="134.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="11" t="n">
         <v>472</v>
       </c>
@@ -29791,7 +29791,7 @@
       <c r="AD308" s="12"/>
       <c r="AE308" s="12"/>
     </row>
-    <row r="309" customFormat="false" ht="322.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="322.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="11" t="n">
         <v>473</v>
       </c>
@@ -29866,7 +29866,7 @@
       <c r="AD309" s="12"/>
       <c r="AE309" s="12"/>
     </row>
-    <row r="310" customFormat="false" ht="134.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="134.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="11" t="n">
         <v>474</v>
       </c>
@@ -29941,7 +29941,7 @@
       <c r="AD310" s="12"/>
       <c r="AE310" s="12"/>
     </row>
-    <row r="311" customFormat="false" ht="80.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="11" t="n">
         <v>475</v>
       </c>
@@ -30016,7 +30016,7 @@
       <c r="AD311" s="12"/>
       <c r="AE311" s="12"/>
     </row>
-    <row r="312" customFormat="false" ht="80.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="11" t="n">
         <v>476</v>
       </c>
@@ -30091,7 +30091,7 @@
       <c r="AD312" s="12"/>
       <c r="AE312" s="12"/>
     </row>
-    <row r="313" customFormat="false" ht="107.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="107.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="11" t="n">
         <v>477</v>
       </c>
@@ -30166,7 +30166,7 @@
       <c r="AD313" s="12"/>
       <c r="AE313" s="12"/>
     </row>
-    <row r="314" customFormat="false" ht="335.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="335.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="11" t="n">
         <v>478</v>
       </c>
@@ -30245,7 +30245,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="375.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="375.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="11" t="n">
         <v>479</v>
       </c>
@@ -30324,7 +30324,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="316" customFormat="false" ht="335.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="335.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="11" t="n">
         <v>480</v>
       </c>
@@ -30403,7 +30403,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="134.3" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="134.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="11" t="n">
         <v>481</v>
       </c>
@@ -30482,7 +30482,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="188.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="188.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="11" t="n">
         <v>482</v>
       </c>
@@ -30561,7 +30561,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="80.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="11" t="n">
         <v>483</v>
       </c>
@@ -30636,7 +30636,7 @@
       <c r="AD319" s="12"/>
       <c r="AE319" s="12"/>
     </row>
-    <row r="320" customFormat="false" ht="174.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="174.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="11" t="n">
         <v>484</v>
       </c>
@@ -30717,7 +30717,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="214.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="214.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="11" t="n">
         <v>485</v>
       </c>
@@ -30796,7 +30796,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="94.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="94.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="11" t="n">
         <v>486</v>
       </c>
@@ -30875,7 +30875,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="148.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="148.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="11" t="n">
         <v>487</v>
       </c>
@@ -30955,18 +30955,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE323">
-    <filterColumn colId="2">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Bakery"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Ice Cream Raw Materials"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <dataValidations count="2">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X2:X249 Z2:AA249" type="list">
       <formula1>"yes,no"</formula1>
@@ -30996,7 +30984,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B250:B282 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31019,7 +31007,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B250:B282 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>